<commit_message>
correcion de matriz sintactica
</commit_message>
<xml_diff>
--- a/recursos/matriz_estados.xlsx
+++ b/recursos/matriz_estados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Kevin Barboza\Documents\Kevin\10mo semestre\compiladores\proyecto_compilador\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Kevin\10mo semestre\compiladores\proyecto_compilador\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B59E06-87C4-483C-A3E9-4B9DBC4DA506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8503FB91-43F4-4720-A8E6-438F44A550E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B964F424-59DC-420D-8D18-139DE96934E4}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9785B6-FC4B-4915-9F11-D05AE974D1C1}">
   <dimension ref="A1:AG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD37" sqref="AD37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="B22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>